<commit_message>
add text files in temp folder
</commit_message>
<xml_diff>
--- a/Test/Test For English Batch.xlsx
+++ b/Test/Test For English Batch.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="291">
   <si>
     <t>Question No</t>
   </si>
@@ -189,21 +189,6 @@
     <t>Table Head D</t>
   </si>
   <si>
-    <t>Judiciable</t>
-  </si>
-  <si>
-    <t>Flexible</t>
-  </si>
-  <si>
-    <t>Non - Judiciable</t>
-  </si>
-  <si>
-    <t>Hard</t>
-  </si>
-  <si>
-    <t>Article 16</t>
-  </si>
-  <si>
     <t>Article 15</t>
   </si>
   <si>
@@ -211,15 +196,6 @@
   </si>
   <si>
     <t>Article 13</t>
-  </si>
-  <si>
-    <t>Which of the following articles of the Constitution of India deals with equality before law?</t>
-  </si>
-  <si>
-    <t>In which article of the Constitution is 'equal protection of law' provided?</t>
-  </si>
-  <si>
-    <t>What are 'Fundamental Rights'?</t>
   </si>
   <si>
     <t>Which of the following is not included in the fundamental right to equality?</t>
@@ -883,6 +859,39 @@
   <si>
     <t>Fulfill:
 ________ without duty is like a man without a shadow.</t>
+  </si>
+  <si>
+    <t>Indus Civilization existed in-</t>
+  </si>
+  <si>
+    <t>The source of knowledge about Harappan culture is:</t>
+  </si>
+  <si>
+    <t>Match List-I with List-II and select the correct answer using the codes given below the lists:</t>
+  </si>
+  <si>
+    <t>Prehistoric age</t>
+  </si>
+  <si>
+    <t>Proto-historic age</t>
+  </si>
+  <si>
+    <t>Historic age</t>
+  </si>
+  <si>
+    <t>Post-Historic age</t>
+  </si>
+  <si>
+    <t>Rock edicts</t>
+  </si>
+  <si>
+    <t>Writing in terracotta seals</t>
+  </si>
+  <si>
+    <t>Archaeological excavations</t>
+  </si>
+  <si>
+    <t>All of the above</t>
   </si>
 </sst>
 </file>
@@ -1253,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AU53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1344,7 +1353,7 @@
         <v>22</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>53</v>
@@ -1430,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>280</v>
       </c>
       <c r="C2" s="3">
         <v>1995</v>
@@ -1449,16 +1458,16 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3" t="s">
-        <v>57</v>
+        <v>283</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>58</v>
+        <v>284</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>59</v>
+        <v>285</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>60</v>
+        <v>286</v>
       </c>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
@@ -1496,27 +1505,27 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="105">
+    <row r="3" spans="1:47" ht="75">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>65</v>
+        <v>281</v>
       </c>
       <c r="C3" s="2">
         <v>1995</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>61</v>
+        <v>287</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>62</v>
+        <v>288</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>63</v>
+        <v>289</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>64</v>
+        <v>290</v>
       </c>
       <c r="AQ3" s="2" t="s">
         <v>25</v>
@@ -1532,27 +1541,27 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="90">
+    <row r="4" spans="1:47" ht="105">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>66</v>
+        <v>282</v>
       </c>
       <c r="C4" s="2">
         <v>1995</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="AQ4" s="2" t="s">
         <v>26</v>
@@ -1573,22 +1582,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2">
         <v>1996</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="AP5" s="6"/>
       <c r="AQ5" s="2" t="s">
@@ -1610,22 +1619,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2">
         <v>1996</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="AQ6" s="2" t="s">
         <v>23</v>
@@ -1646,22 +1655,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2">
         <v>1997</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="AQ7" s="2" t="s">
         <v>25</v>
@@ -1682,7 +1691,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2">
         <v>1997</v>
@@ -1718,22 +1727,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C9" s="2">
         <v>1998</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="AQ9" s="2" t="s">
         <v>23</v>
@@ -1754,7 +1763,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2">
         <v>1999</v>
@@ -1762,16 +1771,16 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="Q10" s="6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="AQ10" s="2" t="s">
         <v>25</v>
@@ -1792,7 +1801,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C11" s="2">
         <v>2006</v>
@@ -1800,16 +1809,16 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="Q11" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="AQ11" s="2" t="s">
         <v>31</v>
@@ -1830,22 +1839,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
@@ -1868,22 +1877,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2">
         <v>2021</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="AQ13" s="2" t="s">
         <v>31</v>
@@ -1903,22 +1912,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C14" s="2">
         <v>2022</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="AQ14" s="2" t="s">
         <v>31</v>
@@ -1938,22 +1947,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C15" s="2">
         <v>2022</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="AQ15" s="2" t="s">
         <v>31</v>
@@ -1973,22 +1982,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C16" s="2">
         <v>2022</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="AQ16" s="2" t="s">
         <v>31</v>
@@ -2008,22 +2017,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C17" s="2">
         <v>2022</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="AQ17" s="2" t="s">
         <v>31</v>
@@ -2043,22 +2052,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C18" s="2">
         <v>2022</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="AQ18" s="2" t="s">
         <v>31</v>
@@ -2078,22 +2087,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C19" s="2">
         <v>2022</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="U19" s="7"/>
       <c r="AQ19" s="2" t="s">
@@ -2114,22 +2123,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C20" s="2">
         <v>2022</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="AQ20" s="2" t="s">
         <v>31</v>
@@ -2149,22 +2158,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C21" s="2">
         <v>2022</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="AQ21" s="2" t="s">
         <v>31</v>
@@ -2184,22 +2193,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C22" s="2">
         <v>2022</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="AQ22" s="2" t="s">
         <v>31</v>
@@ -2219,22 +2228,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2022</v>
+      </c>
+      <c r="Q23" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="2">
-        <v>2022</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="R23" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="AQ23" s="2" t="s">
         <v>31</v>
@@ -2254,22 +2263,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C24" s="2">
         <v>2022</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="R24" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="U24" s="7"/>
       <c r="AQ24" s="2" t="s">
@@ -2290,7 +2299,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C25" s="2">
         <v>2022</v>
@@ -2325,22 +2334,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2022</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="R26" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="T26" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="C26" s="2">
-        <v>2022</v>
-      </c>
-      <c r="Q26" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="R26" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="S26" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="T26" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="AQ26" s="2" t="s">
         <v>31</v>
@@ -2360,22 +2369,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2022</v>
+      </c>
+      <c r="Q27" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C27" s="2">
-        <v>2022</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>163</v>
-      </c>
       <c r="R27" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="U27" s="7"/>
       <c r="AQ27" s="2" t="s">
@@ -2399,22 +2408,22 @@
         <v>2022</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="Q28" s="7" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="U28" s="7"/>
       <c r="AQ28" s="2" t="s">
@@ -2435,22 +2444,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C29" s="2">
         <v>2022</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="R29" s="7" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="S29" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="U29" s="7"/>
       <c r="AQ29" s="2" t="s">
@@ -2471,22 +2480,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C30" s="2">
         <v>2022</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="Q30" s="7" t="s">
         <v>30</v>
@@ -2495,14 +2504,14 @@
         <v>51</v>
       </c>
       <c r="S30" s="7" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="T30" s="7" t="s">
         <v>29</v>
       </c>
       <c r="U30" s="7"/>
       <c r="AP30" s="7" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="AQ30" s="2" t="s">
         <v>31</v>
@@ -2522,22 +2531,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C31" s="2">
         <v>2022</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="R31" s="7" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="U31" s="7"/>
       <c r="AQ31" s="2" t="s">
@@ -2558,22 +2567,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2022</v>
+      </c>
+      <c r="Q32" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="2">
-        <v>2022</v>
-      </c>
-      <c r="Q32" s="7" t="s">
-        <v>194</v>
-      </c>
       <c r="R32" s="7" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="S32" s="7" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="U32" s="7"/>
       <c r="AQ32" s="2" t="s">
@@ -2594,38 +2603,38 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C33" s="2">
         <v>2022</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="R33" s="7" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="T33" s="7" t="s">
         <v>28</v>
       </c>
       <c r="U33" s="7"/>
       <c r="AP33" s="7" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="AQ33" s="2" t="s">
         <v>31</v>
@@ -2645,22 +2654,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C34" s="2">
         <v>2022</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="Q34" s="7" t="s">
         <v>30</v>
@@ -2672,7 +2681,7 @@
         <v>52</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="AQ34" s="2" t="s">
         <v>31</v>
@@ -2692,22 +2701,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C35" s="2">
         <v>2022</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="R35" s="7" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="S35" s="7" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="U35" s="7"/>
       <c r="AQ35" s="2" t="s">
@@ -2728,22 +2737,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C36" s="2">
         <v>2022</v>
       </c>
       <c r="Q36" s="7" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="R36" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="U36" s="7"/>
       <c r="AQ36" s="2" t="s">
@@ -2764,22 +2773,22 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C37" s="2">
         <v>2022</v>
       </c>
       <c r="Q37" s="7" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="R37" s="7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="S37" s="7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="T37" s="7" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="U37" s="7"/>
       <c r="AQ37" s="2" t="s">
@@ -2800,22 +2809,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C38" s="2">
         <v>2022</v>
       </c>
       <c r="Q38" s="7" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="R38" s="7" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="T38" s="8" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="U38" s="8"/>
       <c r="AQ38" s="2" t="s">
@@ -2836,22 +2845,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C39" s="2">
         <v>2022</v>
       </c>
       <c r="Q39" s="7" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="R39" s="7" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="S39" s="7" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="T39" s="7" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="U39" s="7"/>
       <c r="AQ39" s="2" t="s">
@@ -2872,22 +2881,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C40" s="2">
         <v>2022</v>
       </c>
       <c r="Q40" s="7" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="R40" s="7" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="S40" s="7" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="U40" s="7"/>
       <c r="AQ40" s="2" t="s">
@@ -2908,22 +2917,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C41" s="2">
         <v>2022</v>
       </c>
       <c r="Q41" s="7" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="S41" s="7" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="T41" s="7" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="U41" s="7"/>
       <c r="AQ41" s="2" t="s">
@@ -2944,22 +2953,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C42" s="2">
         <v>2022</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="S42" s="7" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="T42" s="7" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="U42" s="7"/>
       <c r="AQ42" s="2" t="s">
@@ -2980,22 +2989,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C43" s="2">
         <v>2022</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="R43" s="7" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="S43" s="7" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="T43" s="7" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="U43" s="7"/>
       <c r="AQ43" s="2" t="s">
@@ -3016,22 +3025,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C44" s="2">
         <v>2022</v>
       </c>
       <c r="Q44" s="7" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="R44" s="7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="S44" s="7" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="T44" s="7" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="U44" s="7"/>
       <c r="AQ44" s="2" t="s">
@@ -3052,22 +3061,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C45" s="2">
         <v>2022</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="AQ45" s="2" t="s">
         <v>31</v>
@@ -3087,22 +3096,22 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C46" s="2">
         <v>2022</v>
       </c>
       <c r="Q46" s="7" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="R46" s="7" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="S46" s="7" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="T46" s="7" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="U46" s="7"/>
       <c r="AQ46" s="2" t="s">
@@ -3123,7 +3132,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C47" s="2">
         <v>2022</v>
@@ -3159,22 +3168,22 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C48" s="2">
         <v>2022</v>
       </c>
       <c r="Q48" s="7" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="R48" s="7" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="S48" s="7" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="T48" s="7" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="U48" s="7"/>
       <c r="AQ48" s="2" t="s">
@@ -3195,22 +3204,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C49" s="2">
         <v>2022</v>
       </c>
       <c r="Q49" s="7" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="R49" s="7" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="S49" s="7" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="U49" s="7"/>
       <c r="AQ49" s="2" t="s">
@@ -3231,25 +3240,25 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C50" s="2">
         <v>2022</v>
       </c>
       <c r="Q50" s="7" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="R50" s="7" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="S50" s="7" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="T50" s="7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="U50" s="7" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="AQ50" s="2" t="s">
         <v>31</v>
@@ -3269,22 +3278,22 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C51" s="2">
         <v>2022</v>
       </c>
       <c r="Q51" s="7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="R51" s="7" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="S51" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="T51" s="7" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="AQ51" s="2" t="s">
         <v>31</v>
@@ -3304,22 +3313,22 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C52" s="2">
         <v>2022</v>
       </c>
       <c r="Q52" s="7" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="R52" s="7" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="S52" s="7" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="T52" s="7" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="AQ52" s="2" t="s">
         <v>31</v>
@@ -3339,22 +3348,22 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C53" s="2">
         <v>2022</v>
       </c>
       <c r="Q53" s="7" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="R53" s="7" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="S53" s="7" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="T53" s="7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="AQ53" s="2" t="s">
         <v>31</v>

</xml_diff>